<commit_message>
checks for catch metadata and updates accordingly
</commit_message>
<xml_diff>
--- a/data-raw/metadata/tisdale_catch_metadata.xlsx
+++ b/data-raw/metadata/tisdale_catch_metadata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-tisdale-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5DBCD7-CD94-4194-9F46-50F27EAECFE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6A5CD9-040B-405D-A387-5D43950B7688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="66">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -232,6 +232,12 @@
   <si>
     <t>Run designation revised after field visit. Levels = c(NA, "Fall", "Spring", "Winter", "Not recorded", "Late fall", "Not applicable (n/a)")
 "Not applicable (n/a)")</t>
+  </si>
+  <si>
+    <t>visitTime2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Date and time of day associated with the end of trap visit. Definition varies based on visitType. </t>
   </si>
 </sst>
 </file>
@@ -534,11 +540,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Z998"/>
+  <dimension ref="A1:Z999"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M14" sqref="M14"/>
+      <selection pane="bottomLeft" activeCell="M11" sqref="M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1106,28 +1112,34 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>41</v>
+        <v>64</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>56</v>
+        <v>65</v>
       </c>
       <c r="C14" s="1" t="s">
-        <v>13</v>
+        <v>39</v>
       </c>
       <c r="D14" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>19</v>
+        <v>39</v>
       </c>
       <c r="F14" s="5"/>
       <c r="G14" s="5"/>
       <c r="H14" s="5"/>
       <c r="I14" s="6"/>
-      <c r="J14" s="5"/>
+      <c r="J14" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="K14" s="6"/>
-      <c r="L14" s="5"/>
-      <c r="M14" s="5"/>
+      <c r="L14" s="10">
+        <v>40366.542060185187</v>
+      </c>
+      <c r="M14" s="10">
+        <v>45540.417326331015</v>
+      </c>
       <c r="N14" s="1"/>
       <c r="O14" s="1"/>
       <c r="P14" s="1"/>
@@ -1144,10 +1156,10 @@
     </row>
     <row r="15" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>13</v>
@@ -1158,14 +1170,14 @@
       <c r="E15" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="3"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="3"/>
-      <c r="M15" s="3"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="5"/>
+      <c r="K15" s="6"/>
+      <c r="L15" s="5"/>
+      <c r="M15" s="5"/>
       <c r="N15" s="1"/>
       <c r="O15" s="1"/>
       <c r="P15" s="1"/>
@@ -1182,10 +1194,10 @@
     </row>
     <row r="16" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>13</v>
@@ -1220,10 +1232,10 @@
     </row>
     <row r="17" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A17" s="4" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
@@ -1258,10 +1270,10 @@
     </row>
     <row r="18" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>36</v>
+        <v>63</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>13</v>
@@ -1295,11 +1307,21 @@
       <c r="Z18" s="1"/>
     </row>
     <row r="19" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="4"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="1"/>
+      <c r="A19" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>19</v>
+      </c>
       <c r="F19" s="3"/>
       <c r="G19" s="3"/>
       <c r="H19" s="3"/>
@@ -1322,20 +1344,20 @@
       <c r="Y19" s="1"/>
       <c r="Z19" s="1"/>
     </row>
-    <row r="20" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="2"/>
       <c r="E20" s="1"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="5"/>
-      <c r="K20" s="6"/>
-      <c r="L20" s="10"/>
-      <c r="M20" s="10"/>
+      <c r="F20" s="3"/>
+      <c r="G20" s="3"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="2"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="2"/>
+      <c r="L20" s="3"/>
+      <c r="M20" s="3"/>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
@@ -1350,7 +1372,7 @@
       <c r="Y20" s="1"/>
       <c r="Z20" s="1"/>
     </row>
-    <row r="21" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -1362,8 +1384,8 @@
       <c r="I21" s="6"/>
       <c r="J21" s="5"/>
       <c r="K21" s="6"/>
-      <c r="L21" s="5"/>
-      <c r="M21" s="5"/>
+      <c r="L21" s="10"/>
+      <c r="M21" s="10"/>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>
@@ -1384,14 +1406,14 @@
       <c r="C22" s="1"/>
       <c r="D22" s="2"/>
       <c r="E22" s="1"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="2"/>
-      <c r="J22" s="3"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="3"/>
-      <c r="M22" s="3"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="5"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="5"/>
+      <c r="K22" s="6"/>
+      <c r="L22" s="5"/>
+      <c r="M22" s="5"/>
       <c r="N22" s="1"/>
       <c r="O22" s="1"/>
       <c r="P22" s="1"/>
@@ -1463,6 +1485,19 @@
       <c r="Z24" s="1"/>
     </row>
     <row r="25" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A25" s="4"/>
+      <c r="B25" s="1"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="1"/>
+      <c r="F25" s="3"/>
+      <c r="G25" s="3"/>
+      <c r="H25" s="3"/>
+      <c r="I25" s="2"/>
+      <c r="J25" s="3"/>
+      <c r="K25" s="2"/>
+      <c r="L25" s="3"/>
+      <c r="M25" s="3"/>
       <c r="N25" s="1"/>
       <c r="O25" s="1"/>
       <c r="P25" s="1"/>
@@ -1478,14 +1513,6 @@
       <c r="Z25" s="1"/>
     </row>
     <row r="26" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="F26" s="3"/>
-      <c r="G26" s="3"/>
-      <c r="H26" s="3"/>
-      <c r="I26" s="2"/>
-      <c r="J26" s="3"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="3"/>
-      <c r="M26" s="3"/>
       <c r="N26" s="1"/>
       <c r="O26" s="1"/>
       <c r="P26" s="1"/>
@@ -1501,19 +1528,27 @@
       <c r="Z26" s="1"/>
     </row>
     <row r="27" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="N27" s="4"/>
-      <c r="O27" s="4"/>
-      <c r="P27" s="4"/>
-      <c r="Q27" s="4"/>
-      <c r="R27" s="4"/>
-      <c r="S27" s="4"/>
-      <c r="T27" s="4"/>
-      <c r="U27" s="4"/>
-      <c r="V27" s="4"/>
-      <c r="W27" s="4"/>
-      <c r="X27" s="4"/>
-      <c r="Y27" s="4"/>
-      <c r="Z27" s="4"/>
+      <c r="F27" s="3"/>
+      <c r="G27" s="3"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="2"/>
+      <c r="J27" s="3"/>
+      <c r="K27" s="2"/>
+      <c r="L27" s="3"/>
+      <c r="M27" s="3"/>
+      <c r="N27" s="1"/>
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1"/>
+      <c r="R27" s="1"/>
+      <c r="S27" s="1"/>
+      <c r="T27" s="1"/>
+      <c r="U27" s="1"/>
+      <c r="V27" s="1"/>
+      <c r="W27" s="1"/>
+      <c r="X27" s="1"/>
+      <c r="Y27" s="1"/>
+      <c r="Z27" s="1"/>
     </row>
     <row r="28" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="N28" s="4"/>
@@ -1531,19 +1566,19 @@
       <c r="Z28" s="4"/>
     </row>
     <row r="29" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="N29" s="1"/>
-      <c r="O29" s="1"/>
-      <c r="P29" s="1"/>
-      <c r="Q29" s="1"/>
-      <c r="R29" s="1"/>
-      <c r="S29" s="1"/>
-      <c r="T29" s="1"/>
-      <c r="U29" s="1"/>
-      <c r="V29" s="1"/>
-      <c r="W29" s="1"/>
-      <c r="X29" s="1"/>
-      <c r="Y29" s="1"/>
-      <c r="Z29" s="1"/>
+      <c r="N29" s="4"/>
+      <c r="O29" s="4"/>
+      <c r="P29" s="4"/>
+      <c r="Q29" s="4"/>
+      <c r="R29" s="4"/>
+      <c r="S29" s="4"/>
+      <c r="T29" s="4"/>
+      <c r="U29" s="4"/>
+      <c r="V29" s="4"/>
+      <c r="W29" s="4"/>
+      <c r="X29" s="4"/>
+      <c r="Y29" s="4"/>
+      <c r="Z29" s="4"/>
     </row>
     <row r="30" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="N30" s="1"/>
@@ -1561,19 +1596,6 @@
       <c r="Z30" s="1"/>
     </row>
     <row r="31" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="4"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="2"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="3"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="2"/>
-      <c r="L31" s="3"/>
-      <c r="M31" s="3"/>
       <c r="N31" s="1"/>
       <c r="O31" s="1"/>
       <c r="P31" s="1"/>
@@ -1673,7 +1695,7 @@
       <c r="Z34" s="1"/>
     </row>
     <row r="35" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A35" s="11"/>
+      <c r="A35" s="4"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="2"/>
@@ -1701,7 +1723,7 @@
       <c r="Z35" s="1"/>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="12"/>
+      <c r="A36" s="11"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="2"/>
@@ -1729,7 +1751,7 @@
       <c r="Z36" s="1"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="11"/>
+      <c r="A37" s="12"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="2"/>
@@ -1757,7 +1779,7 @@
       <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="12"/>
+      <c r="A38" s="11"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="2"/>
@@ -1785,7 +1807,7 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="4"/>
+      <c r="A39" s="12"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="2"/>
@@ -2737,7 +2759,7 @@
       <c r="Z72" s="1"/>
     </row>
     <row r="73" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A73" s="1"/>
+      <c r="A73" s="4"/>
       <c r="B73" s="1"/>
       <c r="C73" s="1"/>
       <c r="D73" s="2"/>
@@ -28664,22 +28686,50 @@
       <c r="Y998" s="1"/>
       <c r="Z998" s="1"/>
     </row>
+    <row r="999" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A999" s="1"/>
+      <c r="B999" s="1"/>
+      <c r="C999" s="1"/>
+      <c r="D999" s="2"/>
+      <c r="E999" s="1"/>
+      <c r="F999" s="3"/>
+      <c r="G999" s="3"/>
+      <c r="H999" s="3"/>
+      <c r="I999" s="2"/>
+      <c r="J999" s="3"/>
+      <c r="K999" s="2"/>
+      <c r="L999" s="3"/>
+      <c r="M999" s="3"/>
+      <c r="N999" s="1"/>
+      <c r="O999" s="1"/>
+      <c r="P999" s="1"/>
+      <c r="Q999" s="1"/>
+      <c r="R999" s="1"/>
+      <c r="S999" s="1"/>
+      <c r="T999" s="1"/>
+      <c r="U999" s="1"/>
+      <c r="V999" s="1"/>
+      <c r="W999" s="1"/>
+      <c r="X999" s="1"/>
+      <c r="Y999" s="1"/>
+      <c r="Z999" s="1"/>
+    </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="A36:A37"/>
+    <mergeCell ref="A38:A39"/>
   </mergeCells>
   <dataValidations count="4">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C55:C998 C31:C43 C1:C24" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C56:C999 C32:C44 C1:C25" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"nominal,ordinal,interval,ratio,dateTime"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E31:E998 E1:E24" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="E32:E999 E1:E25" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"text,enumerated,dateTime,numeric"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F26 F31:F998 F1:F24" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F27 F32:F999 F1:F25" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"ratio,interval"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H26 H31:H998 H1:H24" xr:uid="{00000000-0002-0000-0000-000003000000}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="H27 H32:H999 H1:H25" xr:uid="{00000000-0002-0000-0000-000003000000}">
       <formula1>"natural,whole,integer,real"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
addresses edi issues on make metadata, validates xml, adds note
</commit_message>
<xml_diff>
--- a/data-raw/metadata/tisdale_catch_metadata.xlsx
+++ b/data-raw/metadata/tisdale_catch_metadata.xlsx
@@ -8,20 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-tisdale-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9F6A5CD9-040B-405D-A387-5D43950B7688}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1864CA60-55BB-4B0A-A9CF-AB24EE23B4DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3370" yWindow="2860" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
     <sheet name="code_definitions" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="0"/>
-  <extLst>
-    <ext uri="GoogleSheetsCustomDataVersion1">
-      <go:sheetsCustomData xmlns:go="http://customooxmlschemas.google.com/" r:id="rId6" roundtripDataSignature="AMtx7mjgCtONQL+sZFXm0/U8uf/vdSvo/w=="/>
-    </ext>
-  </extLst>
 </workbook>
 </file>
 
@@ -544,7 +539,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M11" sqref="M11"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -28743,7 +28738,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
adds clean csvs with updated data, checks metadata
</commit_message>
<xml_diff>
--- a/data-raw/metadata/tisdale_catch_metadata.xlsx
+++ b/data-raw/metadata/tisdale_catch_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-tisdale-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1864CA60-55BB-4B0A-A9CF-AB24EE23B4DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D38E651-092E-41DD-8A17-B0BB888F68F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3370" yWindow="2860" windowWidth="19200" windowHeight="11170" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-21315" yWindow="2655" windowWidth="20565" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="70">
   <si>
     <t xml:space="preserve">attribute_name </t>
   </si>
@@ -234,6 +234,18 @@
   <si>
     <t xml:space="preserve">Date and time of day associated with the end of trap visit. Definition varies based on visitType. </t>
   </si>
+  <si>
+    <t>trap_start_date</t>
+  </si>
+  <si>
+    <t>trap_end_date</t>
+  </si>
+  <si>
+    <t>Start date and time of a trapping period. Derived from visitTime and visitTime2 fields, adjusted based on the visitType field</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> End date and time of a trapping period. Derived from visitTime and visitTime2 fields, adjusted based on the visitType field</t>
+  </si>
 </sst>
 </file>
 
@@ -294,7 +306,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -320,6 +332,9 @@
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="22" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -537,9 +552,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="170" zoomScaleNormal="170" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -1340,19 +1355,35 @@
       <c r="Z19" s="1"/>
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="4"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="1"/>
+      <c r="A20" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="3"/>
       <c r="I20" s="2"/>
-      <c r="J20" s="3"/>
+      <c r="J20" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="K20" s="2"/>
-      <c r="L20" s="3"/>
-      <c r="M20" s="3"/>
+      <c r="L20" s="13">
+        <v>40365.542060185187</v>
+      </c>
+      <c r="M20" s="13">
+        <v>45539.417326388888</v>
+      </c>
       <c r="N20" s="1"/>
       <c r="O20" s="1"/>
       <c r="P20" s="1"/>
@@ -1368,19 +1399,35 @@
       <c r="Z20" s="1"/>
     </row>
     <row r="21" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="4"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="1"/>
+      <c r="A21" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>39</v>
+      </c>
       <c r="F21" s="5"/>
       <c r="G21" s="5"/>
       <c r="H21" s="5"/>
       <c r="I21" s="6"/>
-      <c r="J21" s="5"/>
+      <c r="J21" s="5" t="s">
+        <v>40</v>
+      </c>
       <c r="K21" s="6"/>
-      <c r="L21" s="10"/>
-      <c r="M21" s="10"/>
+      <c r="L21" s="13">
+        <v>40365.542060185187</v>
+      </c>
+      <c r="M21" s="13">
+        <v>45539.417326388888</v>
+      </c>
       <c r="N21" s="1"/>
       <c r="O21" s="1"/>
       <c r="P21" s="1"/>

</xml_diff>

<commit_message>
removes lower feather site, writes csvs
</commit_message>
<xml_diff>
--- a/data-raw/metadata/tisdale_catch_metadata.xlsx
+++ b/data-raw/metadata/tisdale_catch_metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Badhia\Documents\git\jpe-tisdale-edi\data-raw\metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D38E651-092E-41DD-8A17-B0BB888F68F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C0152A0-4383-4515-8077-8EEE519C1B73}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21315" yWindow="2655" windowWidth="20565" windowHeight="11175" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5550" yWindow="1780" windowWidth="16860" windowHeight="13080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="attribute" sheetId="1" r:id="rId1"/>
@@ -188,9 +188,6 @@
     <t>Tisdale RST</t>
   </si>
   <si>
-    <t>Name of the sampling site. Levels = c("Tisdale Weir RST", "Lower Feather River RST")</t>
-  </si>
-  <si>
     <t>Work that was done during visit to trap. Levels = c("Continue trapping", "Unplanned restart", "End trapping", "Start trap &amp; begin trapping", "Service/adjust/clean trap", "Drive-by only")</t>
   </si>
   <si>
@@ -245,6 +242,9 @@
   </si>
   <si>
     <t xml:space="preserve"> End date and time of a trapping period. Derived from visitTime and visitTime2 fields, adjusted based on the visitType field</t>
+  </si>
+  <si>
+    <t>Name of the sampling site. Levels = c("Tisdale Weir RST")</t>
   </si>
 </sst>
 </file>
@@ -330,11 +330,11 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -552,9 +552,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A13" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L10" sqref="L10"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.1640625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -633,7 +633,7 @@
         <v>44</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>18</v>
@@ -747,7 +747,7 @@
         <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>13</v>
@@ -823,7 +823,7 @@
         <v>51</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>13</v>
@@ -861,7 +861,7 @@
         <v>24</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>13</v>
@@ -899,7 +899,7 @@
         <v>25</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>13</v>
@@ -1122,10 +1122,10 @@
     </row>
     <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>39</v>
@@ -1169,7 +1169,7 @@
         <v>41</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>13</v>
@@ -1207,7 +1207,7 @@
         <v>42</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>55</v>
+        <v>69</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>13</v>
@@ -1245,7 +1245,7 @@
         <v>43</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>13</v>
@@ -1283,7 +1283,7 @@
         <v>52</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>13</v>
@@ -1356,10 +1356,10 @@
     </row>
     <row r="20" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>39</v>
@@ -1378,10 +1378,10 @@
         <v>40</v>
       </c>
       <c r="K20" s="2"/>
-      <c r="L20" s="13">
+      <c r="L20" s="11">
         <v>40365.542060185187</v>
       </c>
-      <c r="M20" s="13">
+      <c r="M20" s="11">
         <v>45539.417326388888</v>
       </c>
       <c r="N20" s="1"/>
@@ -1400,10 +1400,10 @@
     </row>
     <row r="21" spans="1:26" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A21" s="4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>39</v>
@@ -1422,10 +1422,10 @@
         <v>40</v>
       </c>
       <c r="K21" s="6"/>
-      <c r="L21" s="13">
+      <c r="L21" s="11">
         <v>40365.542060185187</v>
       </c>
-      <c r="M21" s="13">
+      <c r="M21" s="11">
         <v>45539.417326388888</v>
       </c>
       <c r="N21" s="1"/>
@@ -1765,7 +1765,7 @@
       <c r="Z35" s="1"/>
     </row>
     <row r="36" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A36" s="11"/>
+      <c r="A36" s="12"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="2"/>
@@ -1793,7 +1793,7 @@
       <c r="Z36" s="1"/>
     </row>
     <row r="37" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A37" s="12"/>
+      <c r="A37" s="13"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="2"/>
@@ -1821,7 +1821,7 @@
       <c r="Z37" s="1"/>
     </row>
     <row r="38" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A38" s="11"/>
+      <c r="A38" s="12"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="2"/>
@@ -1849,7 +1849,7 @@
       <c r="Z38" s="1"/>
     </row>
     <row r="39" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A39" s="12"/>
+      <c r="A39" s="13"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="2"/>

</xml_diff>